<commit_message>
Updated the wrongly placed data for the sediment data
</commit_message>
<xml_diff>
--- a/All_code_data_visualization/95_pesticide/Ogbeide_et_al_2025 statistical summary and model output.xlsx.xlsx
+++ b/All_code_data_visualization/95_pesticide/Ogbeide_et_al_2025 statistical summary and model output.xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/collins/Downloads/Desktop/Manuscript 2022/pollution_flow/All_code_data_visualization/95_pesticide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBCBFA9-457F-6349-9C78-74926C1F9EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D34BF6-1713-E540-8A04-64A1273A07FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12340" yWindow="760" windowWidth="17460" windowHeight="17980" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6580" yWindow="760" windowWidth="17460" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table content" sheetId="9" r:id="rId1"/>
@@ -700,9 +700,6 @@
     <t>Statistical summary of the physicochemical parameters measured during the treatment phase in both inlet and outlet sections of each treatments</t>
   </si>
   <si>
-    <t>Statistical summary of instream sediment pesticide compounds and their concentrations above limits of quantification (LOQ) in control and low-flow treatments.</t>
-  </si>
-  <si>
     <t>Statistical summary of pesticide compounds and their concentrations above the limits of quantification (LOQ) in daily water samples collected from the river supplying the Riparian Stream Mesocosm (RSM)</t>
   </si>
   <si>
@@ -734,7 +731,7 @@
   </si>
   <si>
     <r>
-      <t>Summary of Generalized Linear Mixed Model (GLMM) results: Response of instream sediment pesticide concentrations (µg/kg) across two sampling weeks, emerging insect abundance (ind. m⁻² day⁻¹) and biomass (mg m⁻² day⁻¹) across five sampling weeks, and spider abundance by flume under Control and Low-Flow Treatments. Significant p-values (</t>
+      <t>Summary of Generalized Linear Mixed Model (GLMM) results: Response of in-stream sediment pesticide concentrations (µg/kg) across two sampling weeks, emerging insect abundance (ind. m⁻² day⁻¹) and biomass (mg m⁻² day⁻¹) across five sampling weeks, and spider abundance by flume under Control and Low-Flow Treatments. Significant p-values (</t>
     </r>
     <r>
       <rPr>
@@ -755,6 +752,9 @@
       </rPr>
       <t>) are shown in bold.</t>
     </r>
+  </si>
+  <si>
+    <t>Statistical summary of in-stream sediment pesticide compounds and their concentrations above limits of quantification (LOQ) in control and low-flow treatments.</t>
   </si>
 </sst>
 </file>
@@ -885,23 +885,23 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1201,34 +1201,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7299C0-EB0C-A84F-9AB8-EF6DE75392CD}">
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:22" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
@@ -1237,26 +1237,26 @@
       <c r="A2" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
@@ -1265,26 +1265,26 @@
       <c r="A3" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
@@ -1317,10 +1317,10 @@
       <c r="A5" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1345,26 +1345,26 @@
       <c r="A6" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
@@ -1373,26 +1373,26 @@
       <c r="A7" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
@@ -1401,26 +1401,26 @@
       <c r="A8" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
+      <c r="B8" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
       <c r="T8" s="2"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
@@ -1429,26 +1429,26 @@
       <c r="A9" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
+      <c r="B9" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
@@ -1457,26 +1457,26 @@
       <c r="A10" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
+      <c r="B10" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
@@ -1485,50 +1485,50 @@
       <c r="A11" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
+      <c r="B11" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
     <row r="12" spans="1:22" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
@@ -1823,17 +1823,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="B1:S1"/>
-    <mergeCell ref="B3:S3"/>
-    <mergeCell ref="B10:S10"/>
-    <mergeCell ref="B11:S11"/>
     <mergeCell ref="B12:S12"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:S6"/>
     <mergeCell ref="B7:S7"/>
     <mergeCell ref="B8:S8"/>
     <mergeCell ref="B9:S9"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="B3:S3"/>
+    <mergeCell ref="B10:S10"/>
+    <mergeCell ref="B11:S11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1843,7 +1843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -3818,8 +3818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40A8812-8F26-2E4E-9144-F8BAB65584AD}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8694,7 +8694,7 @@
     </row>
     <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>0</v>

</xml_diff>